<commit_message>
Updated login paramaterized test Cases
</commit_message>
<xml_diff>
--- a/TestData/OrangeHRM_DDT.xlsx
+++ b/TestData/OrangeHRM_DDT.xlsx
@@ -467,12 +467,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Login Successful</t>
+          <t>Login Failed</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
     </row>

</xml_diff>